<commit_message>
Added Listener and API framework
</commit_message>
<xml_diff>
--- a/src/test/testData/Userdata.xlsx
+++ b/src/test/testData/Userdata.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nataliia_Salo\TAF_Kseniia\testData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nataliia_Salo\TAF_Kseniia\src\test\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7D0FB26-0106-4D84-84C0-ECA0E7893AEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D59BBDB-595B-4B92-AC78-94D74BF106BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>UserID</t>
   </si>
@@ -79,6 +79,9 @@
   </si>
   <si>
     <t>Joe@gmail.com</t>
+  </si>
+  <si>
+    <t>TestUser112</t>
   </si>
 </sst>
 </file>
@@ -418,11 +421,12 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="2" max="2" width="14.33203125" customWidth="1"/>
     <col min="5" max="5" width="20" customWidth="1"/>
     <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
   </cols>
@@ -449,10 +453,10 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>8476458</v>
+        <v>968754</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C2" t="s">
         <v>15</v>
@@ -463,8 +467,8 @@
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F2">
-        <v>754645</v>
+      <c r="F2" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="G2">
         <v>46464376</v>
@@ -523,6 +527,7 @@
     <hyperlink ref="E4" r:id="rId3" xr:uid="{9F2200A2-53B5-4BEB-AB7E-2856E83F6DA3}"/>
     <hyperlink ref="F3" r:id="rId4" xr:uid="{C6619A56-0065-45DA-B3C2-BDFD17B5C951}"/>
     <hyperlink ref="F4" r:id="rId5" xr:uid="{9B568C0B-AEF5-4572-8D4B-00A683456C56}"/>
+    <hyperlink ref="F2" r:id="rId6" xr:uid="{43A89932-2796-424D-8141-988CAD64A451}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>